<commit_message>
Add forward dynamics functions (HandC(), FDcrb())
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="223">
   <si>
     <t>Block</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>verify</t>
+  </si>
+  <si>
+    <t>dimChange</t>
   </si>
 </sst>
 </file>
@@ -2858,10 +2861,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2872,10 +2875,11 @@
     <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="56" customFormat="1">
+    <row r="1" spans="1:7" s="56" customFormat="1">
       <c r="A1" s="56" t="s">
         <v>150</v>
       </c>
@@ -2894,8 +2898,11 @@
       <c r="F1" s="56" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="D2" t="s">
         <v>211</v>
       </c>
@@ -2906,7 +2913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="57" t="s">
         <v>213</v>
       </c>
@@ -2920,7 +2927,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="57" t="s">
         <v>213</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="57" t="s">
         <v>213</v>
       </c>
@@ -2948,7 +2955,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="57" t="s">
         <v>213</v>
       </c>
@@ -2962,7 +2969,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="57" t="s">
         <v>213</v>
       </c>
@@ -2976,7 +2983,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="57" t="s">
         <v>213</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="57" t="s">
         <v>213</v>
       </c>
@@ -3004,7 +3011,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="57" t="s">
         <v>213</v>
       </c>
@@ -3018,7 +3025,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="57" t="s">
         <v>213</v>
       </c>
@@ -3032,7 +3039,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="57" t="s">
         <v>213</v>
       </c>
@@ -3046,7 +3053,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="57" t="s">
         <v>213</v>
       </c>
@@ -3060,7 +3067,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="57" t="s">
         <v>213</v>
       </c>
@@ -3074,7 +3081,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="57" t="s">
         <v>213</v>
       </c>
@@ -3088,7 +3095,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="57" t="s">
         <v>213</v>
       </c>
@@ -3269,25 +3276,31 @@
       </c>
     </row>
     <row r="29" spans="1:6">
+      <c r="A29" s="57" t="s">
+        <v>213</v>
+      </c>
       <c r="D29" t="s">
         <v>215</v>
       </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>3</v>
+      <c r="E29" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:6">
+      <c r="A30" s="57" t="s">
+        <v>213</v>
+      </c>
       <c r="D30" t="s">
         <v>216</v>
       </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30">
-        <v>3</v>
+      <c r="E30" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3321,6 +3334,12 @@
       </c>
       <c r="F33">
         <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
+      <c r="E34" s="38"/>
+      <c r="F34" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FDab(). Basic functions are now complete
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="223">
   <si>
     <t>Block</t>
   </si>
@@ -2864,7 +2864,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3304,41 +3304,40 @@
       </c>
     </row>
     <row r="31" spans="1:6">
+      <c r="A31" s="57" t="s">
+        <v>213</v>
+      </c>
       <c r="D31" t="s">
         <v>217</v>
       </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31">
-        <v>3</v>
+      <c r="E31" s="57" t="s">
+        <v>217</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="D32" t="s">
         <v>218</v>
       </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-      <c r="F32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6">
+    </row>
+    <row r="33" spans="1:6">
       <c r="D33" t="s">
         <v>219</v>
       </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6">
-      <c r="E34" s="38"/>
-      <c r="F34" t="s">
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="57" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="F34" s="57" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.6 FDcrb is symbolic and numeric
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -129,7 +129,7 @@
     <author>Reyes Fabian</author>
   </authors>
   <commentList>
-    <comment ref="F20" authorId="0">
+    <comment ref="F23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0">
+    <comment ref="F30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="244">
   <si>
     <t>Block</t>
   </si>
@@ -691,9 +691,6 @@
     <t>checkConfigurationDMX()</t>
   </si>
   <si>
-    <t>Check the IDs of the currently configured servos</t>
-  </si>
-  <si>
     <t>COMMAND</t>
   </si>
   <si>
@@ -718,9 +715,6 @@
     <t>closedLoopControl</t>
   </si>
   <si>
-    <t>"0.10"</t>
-  </si>
-  <si>
     <t>Function Name</t>
   </si>
   <si>
@@ -851,6 +845,75 @@
   </si>
   <si>
     <t>dimChange</t>
+  </si>
+  <si>
+    <t>parseMessageDMXL()</t>
+  </si>
+  <si>
+    <t>Check the IDs of the currently configured servos on the Duo</t>
+  </si>
+  <si>
+    <t>stateRoll</t>
+  </si>
+  <si>
+    <t>velocityRoll</t>
+  </si>
+  <si>
+    <t>angleFilter</t>
+  </si>
+  <si>
+    <t>velocityFilterFIR</t>
+  </si>
+  <si>
+    <t>velocityFilter</t>
+  </si>
+  <si>
+    <t>v0.5</t>
+  </si>
+  <si>
+    <t>v0.10</t>
+  </si>
+  <si>
+    <t>v0.6</t>
+  </si>
+  <si>
+    <t>v0.7</t>
+  </si>
+  <si>
+    <t>v0.9</t>
+  </si>
+  <si>
+    <t>v0.11</t>
+  </si>
+  <si>
+    <t>v0.12</t>
+  </si>
+  <si>
+    <t>v0.13</t>
+  </si>
+  <si>
+    <t>v0.14</t>
+  </si>
+  <si>
+    <t>v0.16</t>
+  </si>
+  <si>
+    <t>v0.17</t>
+  </si>
+  <si>
+    <t>setupDMXL[]</t>
+  </si>
+  <si>
+    <t>Updated for sympy</t>
+  </si>
+  <si>
+    <t>invPluX</t>
+  </si>
+  <si>
+    <t>invPluXf</t>
+  </si>
+  <si>
+    <t>derRot</t>
   </si>
 </sst>
 </file>
@@ -894,7 +957,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,6 +991,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1064,7 +1133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1172,6 +1241,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2220,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2237,7 +2307,7 @@
     <col min="7" max="7" width="7.5703125" style="42" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" style="42" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="33" customWidth="1"/>
     <col min="11" max="11" width="114.42578125" style="42" bestFit="1" customWidth="1"/>
     <col min="12" max="1029" width="8.7109375"/>
   </cols>
@@ -2250,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>137</v>
@@ -2285,8 +2355,8 @@
       <c r="D2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="42">
-        <v>0.5</v>
+      <c r="E2" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>79</v>
@@ -2300,8 +2370,11 @@
       <c r="D3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="42">
-        <v>0.5</v>
+      <c r="E3" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>10</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>80</v>
@@ -2315,8 +2388,11 @@
       <c r="D4" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="42">
-        <v>0.5</v>
+      <c r="E4" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>13</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>81</v>
@@ -2330,8 +2406,11 @@
       <c r="D5" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
+      <c r="E5" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>239</v>
       </c>
       <c r="K5" s="32" t="s">
         <v>163</v>
@@ -2344,8 +2423,11 @@
       <c r="D6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="42">
-        <v>0.5</v>
+      <c r="E6" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>88</v>
@@ -2356,13 +2438,16 @@
         <v>152</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="42">
-        <v>0.5</v>
+      <c r="E7" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>25</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>89</v>
@@ -2375,482 +2460,530 @@
       <c r="D8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="42">
-        <v>0.5</v>
+      <c r="E8" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="38" customFormat="1">
-      <c r="A9" s="40" t="s">
+    <row r="9" spans="1:11">
+      <c r="B9" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="38" customFormat="1">
+      <c r="A10" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B10" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C10" s="45">
         <v>129</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D10" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="47" t="s">
+      <c r="E10" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="38" customFormat="1">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" s="50">
-        <v>130</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" s="38" customFormat="1">
       <c r="A11" s="53"/>
       <c r="B11" s="54" t="s">
         <v>165</v>
       </c>
       <c r="C11" s="50">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
-      <c r="I11" s="50">
-        <v>0.17</v>
-      </c>
+      <c r="I11" s="50"/>
       <c r="J11" s="55"/>
-      <c r="K11" s="50" t="s">
-        <v>169</v>
+      <c r="K11" s="32" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:11">
+      <c r="A12" s="53"/>
+      <c r="B12" s="54" t="s">
+        <v>165</v>
+      </c>
       <c r="C12" s="50">
-        <v>145</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>91</v>
+        <v>132</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="J12" s="55"/>
+      <c r="K12" s="50" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="C13" s="50"/>
+      <c r="C13" s="50">
+        <v>255</v>
+      </c>
       <c r="D13" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K13" s="32" t="s">
-        <v>162</v>
+        <v>141</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="I13" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="C14" s="50">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="42">
-        <v>0.5</v>
+        <v>29</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="C15" s="50">
-        <v>30</v>
-      </c>
+      <c r="C15" s="50"/>
       <c r="D15" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>103</v>
+        <v>142</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="C16" s="50">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="42">
-        <v>0.5</v>
+        <v>37</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="3:11">
       <c r="C17" s="50">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="42">
-        <v>0.5</v>
+        <v>40</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="3:11">
       <c r="C18" s="50">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="42">
-        <v>0.5</v>
+        <v>42</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="3:11">
       <c r="C19" s="50">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="42">
-        <v>0.5</v>
+        <v>44</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="3:11">
       <c r="C20" s="50">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="42">
-        <v>0.5</v>
+        <v>121</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="3:11">
       <c r="C21" s="50">
+        <v>38</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11">
+      <c r="C22" s="50">
         <v>68</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D22" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11">
+      <c r="C23" s="50">
+        <v>68</v>
+      </c>
+      <c r="D23" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K21" s="1" t="s">
+      <c r="E23" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="3:11">
-      <c r="D22" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11">
-      <c r="D23" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="24" spans="3:11">
       <c r="D24" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="42">
-        <v>0.5</v>
+        <v>58</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="3:11">
       <c r="D25" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11">
+      <c r="D26" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11">
+      <c r="D27" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K25" s="1" t="s">
+      <c r="E27" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11">
-      <c r="D26" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11">
-      <c r="D27" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="28" spans="3:11">
       <c r="D28" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11">
+      <c r="D29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11">
+      <c r="D30" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K28" s="1" t="s">
+      <c r="E30" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K30" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="3:11">
-      <c r="D29" s="14" t="s">
+    <row r="31" spans="3:11">
+      <c r="D31" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="K29" s="1" t="s">
+      <c r="E31" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K31" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="3:11">
-      <c r="C30" s="42">
+    <row r="32" spans="3:11">
+      <c r="C32" s="42">
         <v>200</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D32" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="E30" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="I30" s="42">
-        <v>0.12</v>
-      </c>
-      <c r="K30" s="1" t="s">
+      <c r="E32" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="I32" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="3:11">
-      <c r="C31" s="42">
-        <v>201</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="E31" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="I31" s="42">
-        <v>0.12</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="3:11">
-      <c r="D32" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="E32" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="I32" s="42">
-        <v>0.12</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="33" spans="3:11">
       <c r="C33" s="42">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="E33" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="I33" s="42">
-        <v>0.12</v>
+        <v>156</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>234</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="3:11">
-      <c r="C34" s="50">
-        <v>203</v>
-      </c>
       <c r="D34" s="42" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" s="50">
-        <v>0.6</v>
-      </c>
-      <c r="I34" s="50">
-        <v>0.13</v>
-      </c>
-      <c r="K34" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="I34" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="K34" s="32" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="35" spans="3:11">
       <c r="C35" s="42">
-        <v>204</v>
-      </c>
-      <c r="D35" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="E35" s="50">
-        <v>0.6</v>
-      </c>
-      <c r="I35" s="50">
-        <v>0.13</v>
-      </c>
-      <c r="K35" s="1"/>
+        <v>202</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="I35" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="36" spans="3:11">
       <c r="C36" s="50">
-        <v>205</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="50">
-        <v>0.6</v>
-      </c>
-      <c r="I36" s="50">
-        <v>0.13</v>
+        <v>203</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="I36" s="50" t="s">
+        <v>235</v>
       </c>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="3:11">
       <c r="C37" s="42">
-        <v>206</v>
-      </c>
-      <c r="D37" s="42" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" s="50">
-        <v>0.7</v>
-      </c>
-      <c r="I37" s="42">
-        <v>0.14000000000000001</v>
+        <v>204</v>
+      </c>
+      <c r="D37" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="I37" s="50" t="s">
+        <v>235</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="3:11">
       <c r="C38" s="50">
-        <v>207</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="E38" s="50">
-        <v>0.7</v>
-      </c>
-      <c r="I38" s="42">
-        <v>0.14000000000000001</v>
+        <v>205</v>
+      </c>
+      <c r="D38" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="I38" s="50" t="s">
+        <v>235</v>
       </c>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="3:11">
-      <c r="C39" s="50">
-        <v>208</v>
-      </c>
-      <c r="D39" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="E39" s="50">
-        <v>0.9</v>
-      </c>
-      <c r="I39" s="50">
-        <v>0.16</v>
+      <c r="C39" s="42">
+        <v>206</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="I39" s="42" t="s">
+        <v>236</v>
       </c>
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="3:11">
       <c r="C40" s="50">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="I40" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>143</v>
+        <v>175</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="I40" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="3:11">
+      <c r="C41" s="50">
+        <v>208</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="I41" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="3:11">
+      <c r="D42" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="E42" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11">
+      <c r="D43" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11">
+      <c r="D44" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11">
+      <c r="D45" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11">
+      <c r="D46" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2861,10 +2994,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2875,11 +3008,12 @@
     <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.7109375"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="56" customFormat="1">
+    <row r="1" spans="1:8" s="56" customFormat="1">
       <c r="A1" s="56" t="s">
         <v>150</v>
       </c>
@@ -2887,458 +3021,563 @@
         <v>0</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="G1" s="56" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="E4" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="D2" t="s">
+      <c r="E5" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="57" t="s">
+      <c r="D6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="G11" s="59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="G13" s="59" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" s="59" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="F16" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="F17" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="G22" s="59" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="59" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F24" s="58"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D25" t="s">
+        <v>202</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="G25" s="59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" s="59" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="F28" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="59" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="59" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" s="59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="G31" s="59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" t="s">
         <v>213</v>
       </c>
-      <c r="D3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" s="57" t="s">
+      <c r="E32" s="57" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="57" t="s">
+        <v>213</v>
+      </c>
+      <c r="G32" s="59" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="57" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="F4" s="57" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>184</v>
-      </c>
-      <c r="F5" s="57" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>185</v>
-      </c>
-      <c r="F6" s="57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" t="s">
-        <v>186</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="F7" s="57" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>187</v>
-      </c>
-      <c r="F8" s="57" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>188</v>
-      </c>
-      <c r="F9" s="57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" t="s">
-        <v>189</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>189</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" s="57" t="s">
-        <v>194</v>
-      </c>
-      <c r="F12" s="57" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D13" t="s">
-        <v>195</v>
-      </c>
-      <c r="E13" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="F13" s="57" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" t="s">
-        <v>196</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>196</v>
-      </c>
-      <c r="F14" s="57" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D15" t="s">
-        <v>197</v>
-      </c>
-      <c r="E15" s="57" t="s">
-        <v>197</v>
-      </c>
-      <c r="F15" s="57" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D16" t="s">
-        <v>198</v>
-      </c>
-      <c r="E16" s="57" t="s">
-        <v>198</v>
-      </c>
-      <c r="F16" s="57" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D19" t="s">
-        <v>201</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>201</v>
-      </c>
-      <c r="F19" s="57" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="D20" t="s">
-        <v>202</v>
-      </c>
-      <c r="E20" s="57" t="s">
-        <v>202</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="38" t="s">
+      <c r="D33" t="s">
+        <v>214</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="G33" s="59" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" t="s">
+        <v>215</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" s="57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="D35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="D36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="57" t="s">
         <v>220</v>
       </c>
-      <c r="D21" t="s">
-        <v>203</v>
-      </c>
-      <c r="E21" t="s">
-        <v>203</v>
-      </c>
-      <c r="F21" s="58"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D22" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>204</v>
-      </c>
-      <c r="F22" s="57" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D23" t="s">
-        <v>205</v>
-      </c>
-      <c r="E23" s="57" t="s">
-        <v>205</v>
-      </c>
-      <c r="F23" s="57" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" t="s">
-        <v>206</v>
-      </c>
-      <c r="E24" s="57" t="s">
-        <v>206</v>
-      </c>
-      <c r="F24" s="57" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" t="s">
-        <v>207</v>
-      </c>
-      <c r="E25" s="57" t="s">
-        <v>207</v>
-      </c>
-      <c r="F25" s="57" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D26" t="s">
-        <v>208</v>
-      </c>
-      <c r="E26" s="57" t="s">
-        <v>208</v>
-      </c>
-      <c r="F26" s="57" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D27" t="s">
-        <v>209</v>
-      </c>
-      <c r="E27" s="57" t="s">
-        <v>209</v>
-      </c>
-      <c r="F27" s="57" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D28" t="s">
-        <v>214</v>
-      </c>
-      <c r="E28" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="F28" s="57" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" t="s">
-        <v>215</v>
-      </c>
-      <c r="E29" s="57" t="s">
-        <v>215</v>
-      </c>
-      <c r="F29" s="57" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D30" t="s">
-        <v>216</v>
-      </c>
-      <c r="E30" s="57" t="s">
-        <v>216</v>
-      </c>
-      <c r="F30" s="57" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" t="s">
-        <v>217</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>217</v>
-      </c>
-      <c r="F31" s="57" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="D32" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="D33" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="57" t="s">
-        <v>222</v>
-      </c>
-      <c r="F34" s="57" t="s">
-        <v>222</v>
+      <c r="F37" s="57" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All basic algorithms both numerical and symbolic
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="244">
   <si>
     <t>Block</t>
   </si>
@@ -2997,7 +2997,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3339,7 +3339,7 @@
       <c r="F21" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="59" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3553,6 +3553,9 @@
         <v>215</v>
       </c>
       <c r="F34" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="G34" s="59" t="s">
         <v>215</v>
       </c>
     </row>

</xml_diff>